<commit_message>
The plugin now returns an array of objects. Each object represents a row.
</commit_message>
<xml_diff>
--- a/tests/Book1.xlsx
+++ b/tests/Book1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\repos\gulp-sheet2json\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="13110" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="13110"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>a</t>
   </si>
@@ -196,12 +201,15 @@
   </si>
   <si>
     <t>d17</t>
+  </si>
+  <si>
+    <t>ende</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -243,12 +251,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -290,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,7 +336,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,11 +547,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="A1:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -571,9 +582,6 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="B3">
         <v>2</v>
       </c>
@@ -608,17 +616,11 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
       <c r="C6">
         <v>5</v>
       </c>
@@ -664,9 +666,6 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -675,9 +674,6 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
       <c r="D10">
         <v>9</v>
       </c>
@@ -686,9 +682,6 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
       <c r="C11">
         <v>10</v>
       </c>
@@ -714,9 +707,6 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
       <c r="C13">
         <v>12</v>
       </c>
@@ -734,8 +724,8 @@
       <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14">
-        <v>13</v>
+      <c r="D14" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -747,11 +737,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -974,7 +964,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- columns where the headere is starting with a exclamation mark will be ignored.
- some cleanup
- some restructuring
</commit_message>
<xml_diff>
--- a/tests/Book1.xlsx
+++ b/tests/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\repos\gulp-sheet2json\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\repos\gulp-sheets2json\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>a</t>
   </si>
@@ -219,6 +219,21 @@
   </si>
   <si>
     <t>dsdas</t>
+  </si>
+  <si>
+    <t>!ddasda</t>
+  </si>
+  <si>
+    <t>fsd</t>
+  </si>
+  <si>
+    <t>fdf</t>
+  </si>
+  <si>
+    <t>fsdf</t>
+  </si>
+  <si>
+    <t>!a</t>
   </si>
 </sst>
 </file>
@@ -562,9 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -573,7 +586,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -583,6 +596,9 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -615,6 +631,9 @@
       <c r="D3">
         <v>2</v>
       </c>
+      <c r="G3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -643,6 +662,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -685,6 +707,9 @@
       <c r="D8">
         <v>7</v>
       </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -699,6 +724,9 @@
       <c r="D9">
         <v>1</v>
       </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
       <c r="J9" t="s">
         <v>63</v>
       </c>
@@ -727,6 +755,9 @@
       <c r="D11">
         <v>10</v>
       </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -752,6 +783,9 @@
       <c r="D13">
         <v>12</v>
       </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -765,6 +799,9 @@
       </c>
       <c r="D14" t="s">
         <v>60</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>